<commit_message>
renamed Guide to docs, added a picture to the readme.md
</commit_message>
<xml_diff>
--- a/Hardware/Controllers/Controller boards/Component list.xlsx
+++ b/Hardware/Controllers/Controller boards/Component list.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcos\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DIYVR\Hardware\Controllers\Controller boards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C39C68D5-6F37-4230-9BCE-11DAE3D0CAC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85BF7B72-0EFD-40DC-B56C-1E30138C4421}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{A137BAAF-7862-4BF4-A60E-98AAC3B3EB8C}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -631,7 +631,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1026,8 +1026,9 @@
     <hyperlink ref="F11" r:id="rId1" xr:uid="{0CAA32BD-3C98-4D35-B6E1-4E121383799B}"/>
     <hyperlink ref="F14" r:id="rId2" xr:uid="{DEF11CC6-758F-42F7-84F9-5742784649D8}"/>
     <hyperlink ref="F15" r:id="rId3" xr:uid="{3A99AF93-674F-410A-A659-D070FC4777E1}"/>
+    <hyperlink ref="F26" r:id="rId4" xr:uid="{9C2D9F87-70A7-4C3B-913D-0099C14CDDF0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>